<commit_message>
rm duplicated update for TX
</commit_message>
<xml_diff>
--- a/data/2020-10-01/texas.xlsx
+++ b/data/2020-10-01/texas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdavis197\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CHS-COMMON\COVID Data Book\Daily updates\20201002\_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42291E95-029C-4620-905D-BE814CAE7503}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3DECA725-5639-434A-A406-86E78A4365E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="806" activeTab="5" xr2:uid="{A6E7ED99-6879-4496-BF23-313330724014}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12230" tabRatio="806" xr2:uid="{A6E7ED99-6879-4496-BF23-313330724014}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases by Age Group" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Fatalities by Gender" sheetId="7" r:id="rId5"/>
     <sheet name="Fatalities by Race-Ethnicity" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -548,16 +548,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBBE98AD-F551-4399-A212-2161860B6EB7}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -568,139 +566,151 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C2" s="12">
-        <v>3.3764247206521537E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <f>B2/$B$15</f>
+        <v>3.4363629681355432E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>847</v>
+        <v>883</v>
       </c>
       <c r="C3" s="12">
-        <v>1.5800175350234112E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C3:C15" si="0">B3/$B$15</f>
+        <v>1.6226248667720239E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>2242</v>
+        <v>2320</v>
       </c>
       <c r="C4" s="12">
-        <v>4.1822896263547668E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>4.2632952331948991E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>10307</v>
+        <v>10476</v>
       </c>
       <c r="C5" s="12">
-        <v>0.19226966627492678</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.19250983130581792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>11406</v>
+        <v>11559</v>
       </c>
       <c r="C6" s="12">
-        <v>0.21277072024175947</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.21241133448491309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>10329</v>
+        <v>10446</v>
       </c>
       <c r="C7" s="12">
-        <v>0.19268006043986793</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.1919585431291117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="4">
-        <v>9007</v>
+        <v>9146</v>
       </c>
       <c r="C8" s="12">
-        <v>0.16801910198294998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.16806938880517475</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="4">
-        <v>3341</v>
+        <v>3388</v>
       </c>
       <c r="C9" s="12">
-        <v>6.2323950230380364E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>6.2258811422691018E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>2277</v>
+        <v>2304</v>
       </c>
       <c r="C10" s="12">
-        <v>4.2475796071408584E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>4.2338931971038996E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="4">
-        <v>1367</v>
+        <v>1379</v>
       </c>
       <c r="C11" s="12">
-        <v>2.5500401067024829E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>2.5340879855930021E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="C12" s="12">
-        <v>1.6490383718544221E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>1.6373258848175237E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="4">
-        <v>1400</v>
+        <v>1420</v>
       </c>
       <c r="C13" s="12">
-        <v>2.6115992314436547E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>2.609430703076188E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -708,17 +718,20 @@
         <v>19</v>
       </c>
       <c r="C14" s="12">
-        <v>3.5443132426735314E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>3.491491785806167E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1">
-        <v>53607</v>
+        <f>SUM(B2:B14)</f>
+        <v>54418</v>
       </c>
       <c r="C15" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -731,13 +744,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB138E10-A78A-4DC8-A42A-79AF36BFE66D}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -748,47 +759,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="4">
-        <v>18135</v>
+        <v>18533</v>
       </c>
       <c r="C2" s="12">
-        <v>0.33829537187307629</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <f>B2/$B$5</f>
+        <v>0.3405674592965563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4">
-        <v>34567</v>
+        <v>34992</v>
       </c>
       <c r="C3" s="12">
-        <v>0.64482250452366296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C3:C5" si="0">B3/$B$5</f>
+        <v>0.64302252931015469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4">
-        <v>905</v>
+        <v>893</v>
       </c>
       <c r="C4" s="12">
-        <v>1.6882123603260767E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>1.6410011393288987E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>53607</v>
+        <f>SUM(B2:B4)</f>
+        <v>54418</v>
       </c>
       <c r="C5" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -801,16 +817,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958BDC2E-149A-4610-AE3E-2ED1092370C8}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -821,40 +835,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="4">
-        <v>801</v>
+        <v>812</v>
       </c>
       <c r="C2" s="12">
-        <v>1.4942078459902624E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <f>B2/$B$8</f>
+        <v>1.4921533316182145E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="4">
-        <v>8888</v>
+        <v>9027</v>
       </c>
       <c r="C3" s="12">
-        <v>0.16579924263622289</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C3:C8" si="0">B3/$B$8</f>
+        <v>0.16588261237090668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="4">
-        <v>21204</v>
+        <v>21472</v>
       </c>
       <c r="C4" s="12">
-        <v>0.39554535788236611</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.39457532434121062</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -862,39 +879,44 @@
         <v>242</v>
       </c>
       <c r="C5" s="12">
-        <v>4.5143358143526031E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>4.4470579587636448E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4">
-        <v>15977</v>
+        <v>16358</v>
       </c>
       <c r="C6" s="12">
-        <v>0.29803943514839482</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.30059906648535412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="4">
-        <v>6495</v>
+        <v>6507</v>
       </c>
       <c r="C7" s="12">
-        <v>0.12115955005876099</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.11957440552758279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>53607</v>
+        <f>SUM(B2:B7)</f>
+        <v>54418</v>
       </c>
       <c r="C8" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -910,16 +932,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F742947-EAB5-4DCC-A1CA-1F4AA7362BD3}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>27</v>
       </c>
@@ -930,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -938,10 +958,11 @@
         <v>3</v>
       </c>
       <c r="C2" s="12">
-        <v>1.9526165061181983E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <f>B2/$B$15</f>
+        <v>1.8873859704309531E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -949,120 +970,131 @@
         <v>6</v>
       </c>
       <c r="C3" s="12">
-        <v>3.9052330122363966E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C3:C15" si="0">B3/$B$15</f>
+        <v>3.7747719408619062E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" s="12">
-        <v>1.0413954699297059E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>1.1324315822585718E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C5" s="12">
-        <v>6.3785472533194479E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>6.4171122994652408E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="C6" s="12">
-        <v>1.8484769591252278E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>1.8748033972947466E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>856</v>
+        <v>893</v>
       </c>
       <c r="C7" s="12">
-        <v>5.5714657641239264E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>5.6181189053161371E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="4">
-        <v>1885</v>
+        <v>1952</v>
       </c>
       <c r="C8" s="12">
-        <v>0.12268940380109347</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.12280591380937401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="4">
-        <v>1474</v>
+        <v>1523</v>
       </c>
       <c r="C9" s="12">
-        <v>9.5938557667274146E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>9.5816294432211388E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>1803</v>
+        <v>1851</v>
       </c>
       <c r="C10" s="12">
-        <v>0.11735225201770372</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.11645171437558981</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="4">
-        <v>2001</v>
+        <v>2082</v>
       </c>
       <c r="C11" s="12">
-        <v>0.13023952095808383</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.13098458634790816</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <v>1882</v>
+        <v>1950</v>
       </c>
       <c r="C12" s="12">
-        <v>0.12249414215048164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.12268008807801195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="4">
-        <v>5056</v>
+        <v>5217</v>
       </c>
       <c r="C13" s="12">
-        <v>0.32908096849778701</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.32821642025794273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -1070,17 +1102,20 @@
         <v>0</v>
       </c>
       <c r="C14" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="8">
-        <v>15364</v>
+        <f>SUM(B2:B14)</f>
+        <v>15895</v>
       </c>
       <c r="C15" s="15">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1093,13 +1128,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92BAF56-3443-4211-AC39-FD818DE6BEEB}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1110,29 +1143,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="7">
-        <v>6411</v>
+        <v>6642</v>
       </c>
       <c r="C2" s="12">
-        <v>0.41727414735745899</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <f>B2/$B$5</f>
+        <v>0.417867253853413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="7">
-        <v>8953</v>
+        <v>9253</v>
       </c>
       <c r="C3" s="12">
-        <v>0.58272585264254095</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C3:C5" si="0">B3/$B$5</f>
+        <v>0.58213274614658694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1140,17 +1175,20 @@
         <v>0</v>
       </c>
       <c r="C4" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>15364</v>
+        <f>SUM(B2:B4)</f>
+        <v>15895</v>
       </c>
       <c r="C5" s="16">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1163,16 +1201,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5030A505-56A3-4E91-AD33-A7ADAD482E9C}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1183,86 +1219,93 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="10">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="C2" s="12">
-        <v>1.8745118458734705E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <f>B2/$B$8</f>
+        <v>1.8559295375904374E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="9">
-        <v>1738</v>
+        <v>1774</v>
       </c>
       <c r="C3" s="12">
-        <v>0.11312158292111429</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C3:C8" si="0">B3/$B$8</f>
+        <v>0.11160742371815036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="10">
-        <v>8618</v>
+        <v>8916</v>
       </c>
       <c r="C4" s="12">
-        <v>0.56092163499088776</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.56093111041207933</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="10">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C5" s="12">
-        <v>5.337151783389742E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>5.4734193142497644E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4">
-        <v>4629</v>
+        <v>4813</v>
       </c>
       <c r="C6" s="12">
-        <v>0.30128872689403802</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0.3027996225228059</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="12">
-        <v>5.8578495183545952E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>6.2912865681031768E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2">
-        <v>15364</v>
+        <v>15895</v>
       </c>
       <c r="C8" s="16">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B7">
-    <sortCondition ref="A2:A7"/>
+  <sortState ref="B18:C23">
+    <sortCondition ref="B18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>